<commit_message>
cierre 13 Sept 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE    ZAVALETA  SEPTIEMBRE   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #09 SEPTIEMBRE 2022/BALANCE    ZAVALETA  SEPTIEMBRE   2022.xlsx
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2273" uniqueCount="1244">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -4607,6 +4607,9 @@
   <si>
     <t xml:space="preserve">VENTAS ZAVALETA DEV. DE PRESTAMO A CENTRAL </t>
   </si>
+  <si>
+    <t xml:space="preserve">DEPOSITAR  A NORMA LEDO PARRA </t>
+  </si>
 </sst>
 </file>
 
@@ -4621,7 +4624,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="75" x14ac:knownFonts="1">
+  <fonts count="76" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5221,6 +5224,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="28">
     <fill>
@@ -5386,7 +5397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="110">
+  <borders count="109">
     <border>
       <left/>
       <right/>
@@ -6557,32 +6568,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="mediumDashDot">
-        <color auto="1"/>
-      </right>
-      <top style="mediumDashDot">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="mediumDashDot">
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="mediumDashDot">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="mediumDashDot">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="mediumDashDot">
         <color auto="1"/>
@@ -6743,12 +6732,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="899">
+  <cellXfs count="905">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -7840,19 +7838,19 @@
     </xf>
     <xf numFmtId="44" fontId="55" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="100" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="98" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="101" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="99" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8056,7 +8054,7 @@
     <xf numFmtId="44" fontId="2" fillId="18" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="0" borderId="104" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="48" fillId="0" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8171,11 +8169,11 @@
     <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="103" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="104" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="105" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="106" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="107" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="108" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="109" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -8269,6 +8267,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="21" borderId="86" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8341,76 +8372,10 @@
     <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8454,6 +8419,39 @@
     </xf>
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -8617,7 +8615,7 @@
     <xf numFmtId="44" fontId="33" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="22" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="22" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="62" fillId="3" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8644,59 +8642,11 @@
     <xf numFmtId="44" fontId="33" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="61" fillId="0" borderId="95" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="61" fillId="0" borderId="97" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="14" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="103" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="23" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="62" fillId="16" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8716,6 +8666,72 @@
     <xf numFmtId="165" fontId="62" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="14" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="18" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="101" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="23" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="23" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="61" fillId="0" borderId="96" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="61" fillId="0" borderId="108" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="24" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -8725,9 +8741,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FF66FFFF"/>
@@ -13688,8 +13704,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
@@ -13697,7 +13713,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -13706,8 +13722,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3924300" y="3943350"/>
-          <a:ext cx="2190750" cy="781050"/>
+          <a:off x="3038475" y="3933825"/>
+          <a:ext cx="2600325" cy="723900"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -14030,23 +14046,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
-      <c r="C1" s="776" t="s">
+      <c r="B1" s="750"/>
+      <c r="C1" s="752" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="777"/>
-      <c r="E1" s="777"/>
-      <c r="F1" s="777"/>
-      <c r="G1" s="777"/>
-      <c r="H1" s="777"/>
-      <c r="I1" s="777"/>
-      <c r="J1" s="777"/>
-      <c r="K1" s="777"/>
-      <c r="L1" s="777"/>
-      <c r="M1" s="777"/>
+      <c r="D1" s="753"/>
+      <c r="E1" s="753"/>
+      <c r="F1" s="753"/>
+      <c r="G1" s="753"/>
+      <c r="H1" s="753"/>
+      <c r="I1" s="753"/>
+      <c r="J1" s="753"/>
+      <c r="K1" s="753"/>
+      <c r="L1" s="753"/>
+      <c r="M1" s="753"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14056,17 +14072,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -14080,14 +14096,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14097,10 +14113,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="755" t="s">
+      <c r="P4" s="766" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="756"/>
+      <c r="Q4" s="767"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -15541,11 +15557,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="757">
+      <c r="M39" s="768">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="759">
+      <c r="N39" s="770">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -15571,8 +15587,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="758"/>
-      <c r="N40" s="760"/>
+      <c r="M40" s="769"/>
+      <c r="N40" s="771"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -15787,29 +15803,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="761" t="s">
+      <c r="H52" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="762"/>
+      <c r="I52" s="773"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="763">
+      <c r="K52" s="774">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="764"/>
-      <c r="M52" s="765">
+      <c r="L52" s="775"/>
+      <c r="M52" s="776">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="766"/>
+      <c r="N52" s="777"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="767" t="s">
+      <c r="D53" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="767"/>
+      <c r="E53" s="778"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -15820,22 +15836,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="767" t="s">
+      <c r="D54" s="778" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="767"/>
+      <c r="E54" s="778"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="768" t="s">
+      <c r="I54" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="769"/>
-      <c r="K54" s="770">
+      <c r="J54" s="780"/>
+      <c r="K54" s="781">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="771"/>
+      <c r="L54" s="782"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -15868,11 +15884,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="772">
+      <c r="K56" s="783">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="773"/>
+      <c r="L56" s="784"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -15889,22 +15905,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="750" t="s">
+      <c r="D58" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="751"/>
+      <c r="E58" s="762"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="752" t="s">
+      <c r="I58" s="763" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="753"/>
-      <c r="K58" s="754">
+      <c r="J58" s="764"/>
+      <c r="K58" s="765">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="754"/>
+      <c r="L58" s="765"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -16048,12 +16064,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -16068,6 +16078,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -18926,7 +18942,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>451</v>
       </c>
@@ -18942,7 +18958,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -18952,21 +18968,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -18984,14 +19000,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -19001,15 +19017,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19060,8 +19076,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19824,7 +19840,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -19876,7 +19892,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -19925,8 +19941,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -20026,8 +20042,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -20082,8 +20098,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -20131,8 +20147,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20181,8 +20197,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20230,9 +20246,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20280,9 +20296,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20614,11 +20630,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="806">
+      <c r="M36" s="795">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="808">
+      <c r="N36" s="797">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -20651,8 +20667,8 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="807"/>
-      <c r="N37" s="809"/>
+      <c r="M37" s="796"/>
+      <c r="N37" s="798"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -21339,26 +21355,26 @@
       <c r="A68" s="98"/>
       <c r="B68" s="99"/>
       <c r="C68" s="1"/>
-      <c r="H68" s="761" t="s">
+      <c r="H68" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="762"/>
+      <c r="I68" s="773"/>
       <c r="J68" s="100"/>
-      <c r="K68" s="763">
+      <c r="K68" s="774">
         <f>I66+L66</f>
         <v>314868.39999999997</v>
       </c>
-      <c r="L68" s="796"/>
+      <c r="L68" s="801"/>
       <c r="M68" s="272"/>
       <c r="N68" s="272"/>
       <c r="P68" s="34"/>
       <c r="Q68" s="13"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D69" s="767" t="s">
+      <c r="D69" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="767"/>
+      <c r="E69" s="778"/>
       <c r="F69" s="312">
         <f>F66-K68-C66</f>
         <v>1594593.8500000003</v>
@@ -21367,22 +21383,22 @@
       <c r="J69" s="103"/>
     </row>
     <row r="70" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D70" s="797" t="s">
+      <c r="D70" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E70" s="797"/>
+      <c r="E70" s="802"/>
       <c r="F70" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I70" s="768" t="s">
+      <c r="I70" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J70" s="769"/>
-      <c r="K70" s="770">
+      <c r="J70" s="780"/>
+      <c r="K70" s="781">
         <f>F72+F73+F74</f>
         <v>1938640.11</v>
       </c>
-      <c r="L70" s="770"/>
+      <c r="L70" s="781"/>
       <c r="M70" s="404"/>
       <c r="N70" s="404"/>
       <c r="O70" s="404"/>
@@ -21423,11 +21439,11 @@
         <v>15</v>
       </c>
       <c r="J72" s="109"/>
-      <c r="K72" s="772">
+      <c r="K72" s="783">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L72" s="773"/>
+      <c r="L72" s="784"/>
     </row>
     <row r="73" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D73" s="110" t="s">
@@ -21444,22 +21460,22 @@
       <c r="C74" s="112">
         <v>44647</v>
       </c>
-      <c r="D74" s="750" t="s">
+      <c r="D74" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="751"/>
+      <c r="E74" s="762"/>
       <c r="F74" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I74" s="752" t="s">
+      <c r="I74" s="763" t="s">
         <v>198</v>
       </c>
-      <c r="J74" s="753"/>
-      <c r="K74" s="754">
+      <c r="J74" s="764"/>
+      <c r="K74" s="765">
         <f>K70+K72</f>
         <v>672071.66000000015</v>
       </c>
-      <c r="L74" s="754"/>
+      <c r="L74" s="765"/>
     </row>
     <row r="75" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C75" s="114"/>
@@ -21606,21 +21622,6 @@
     <sortCondition ref="B34:B42"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M39:N39"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -21636,6 +21637,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:L70"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24248,7 +24264,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>620</v>
       </c>
@@ -24264,7 +24280,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -24274,21 +24290,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -24306,14 +24322,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -24323,15 +24339,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24382,8 +24398,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25142,7 +25158,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -25194,7 +25210,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -25243,8 +25259,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -25341,8 +25357,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -25397,8 +25413,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -25444,8 +25460,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -25496,8 +25512,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -25548,9 +25564,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25600,9 +25616,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26206,11 +26222,11 @@
       <c r="L41" s="624">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="806">
+      <c r="M41" s="795">
         <f>SUM(M5:M40)</f>
         <v>2479367.6100000003</v>
       </c>
-      <c r="N41" s="806">
+      <c r="N41" s="795">
         <f>SUM(N5:N40)</f>
         <v>1195667</v>
       </c>
@@ -26248,8 +26264,8 @@
       <c r="L42" s="627">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="807"/>
-      <c r="N42" s="807"/>
+      <c r="M42" s="796"/>
+      <c r="N42" s="796"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="861"/>
     </row>
@@ -26936,26 +26952,26 @@
       <c r="A70" s="98"/>
       <c r="B70" s="99"/>
       <c r="C70" s="1"/>
-      <c r="H70" s="761" t="s">
+      <c r="H70" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="762"/>
+      <c r="I70" s="773"/>
       <c r="J70" s="100"/>
-      <c r="K70" s="763">
+      <c r="K70" s="774">
         <f>I68+L68</f>
         <v>428155.54000000004</v>
       </c>
-      <c r="L70" s="796"/>
+      <c r="L70" s="801"/>
       <c r="M70" s="272"/>
       <c r="N70" s="272"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="13"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D71" s="767" t="s">
+      <c r="D71" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E71" s="767"/>
+      <c r="E71" s="778"/>
       <c r="F71" s="312">
         <f>F68-K70-C68</f>
         <v>1631087.67</v>
@@ -26965,22 +26981,22 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D72" s="797" t="s">
+      <c r="D72" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="797"/>
+      <c r="E72" s="802"/>
       <c r="F72" s="111">
         <v>-1884975.46</v>
       </c>
-      <c r="I72" s="768" t="s">
+      <c r="I72" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J72" s="769"/>
-      <c r="K72" s="770">
+      <c r="J72" s="780"/>
+      <c r="K72" s="781">
         <f>F74+F75+F76</f>
         <v>1777829.89</v>
       </c>
-      <c r="L72" s="770"/>
+      <c r="L72" s="781"/>
       <c r="M72" s="404"/>
       <c r="N72" s="404"/>
       <c r="O72" s="404"/>
@@ -27021,11 +27037,11 @@
         <v>15</v>
       </c>
       <c r="J74" s="109"/>
-      <c r="K74" s="772">
+      <c r="K74" s="783">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L74" s="773"/>
+      <c r="L74" s="784"/>
       <c r="P74" s="34"/>
     </row>
     <row r="75" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -27044,22 +27060,22 @@
       <c r="C76" s="112">
         <v>44682</v>
       </c>
-      <c r="D76" s="750" t="s">
+      <c r="D76" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E76" s="751"/>
+      <c r="E76" s="762"/>
       <c r="F76" s="113">
         <v>2112071.92</v>
       </c>
-      <c r="I76" s="752" t="s">
+      <c r="I76" s="763" t="s">
         <v>852</v>
       </c>
-      <c r="J76" s="753"/>
-      <c r="K76" s="754">
+      <c r="J76" s="764"/>
+      <c r="K76" s="765">
         <f>K72+K74</f>
         <v>-14987.790000000037</v>
       </c>
-      <c r="L76" s="754"/>
+      <c r="L76" s="765"/>
       <c r="P76" s="34"/>
     </row>
     <row r="77" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
@@ -27219,21 +27235,6 @@
     <sortCondition ref="J47:J67"/>
   </sortState>
   <mergeCells count="30">
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -27249,6 +27250,21 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30438,7 +30454,7 @@
   <dimension ref="B1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30452,11 +30468,11 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="893" t="s">
+      <c r="B2" s="877" t="s">
         <v>1242</v>
       </c>
-      <c r="C2" s="894"/>
-      <c r="D2" s="895"/>
+      <c r="C2" s="878"/>
+      <c r="D2" s="879"/>
       <c r="F2" s="867" t="s">
         <v>1241</v>
       </c>
@@ -30464,9 +30480,9 @@
       <c r="H2" s="869"/>
     </row>
     <row r="3" spans="2:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="896"/>
-      <c r="C3" s="897"/>
-      <c r="D3" s="898"/>
+      <c r="B3" s="880"/>
+      <c r="C3" s="881"/>
+      <c r="D3" s="882"/>
       <c r="F3" s="870"/>
       <c r="G3" s="871"/>
       <c r="H3" s="872"/>
@@ -30635,17 +30651,27 @@
       <c r="C14" s="529"/>
     </row>
     <row r="15" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="877" t="s">
+      <c r="C15" s="875" t="s">
         <v>749</v>
       </c>
-      <c r="D15" s="875">
+      <c r="D15" s="897">
         <f>D11-D13</f>
         <v>-69877</v>
       </c>
+      <c r="E15" s="899" t="s">
+        <v>1243</v>
+      </c>
+      <c r="F15" s="900"/>
+      <c r="G15" s="900"/>
+      <c r="H15" s="901"/>
     </row>
     <row r="16" spans="2:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="878"/>
-      <c r="D16" s="876"/>
+      <c r="C16" s="876"/>
+      <c r="D16" s="898"/>
+      <c r="E16" s="902"/>
+      <c r="F16" s="903"/>
+      <c r="G16" s="903"/>
+      <c r="H16" s="904"/>
     </row>
     <row r="17" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C17" s="866" t="s">
@@ -30654,13 +30680,14 @@
       <c r="D17" s="866"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F2:H3"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E15:H16"/>
   </mergeCells>
   <pageMargins left="0.19" right="0.13" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30709,7 +30736,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>752</v>
       </c>
@@ -30725,7 +30752,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -30735,21 +30762,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -30771,14 +30798,14 @@
       <c r="D4" s="18">
         <v>44682</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -30788,15 +30815,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
       <c r="U4" s="34"/>
       <c r="V4" s="128"/>
-      <c r="W4" s="885"/>
-      <c r="X4" s="885"/>
+      <c r="W4" s="883"/>
+      <c r="X4" s="883"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -30850,8 +30877,8 @@
       <c r="S5" s="324"/>
       <c r="U5" s="34"/>
       <c r="V5" s="128"/>
-      <c r="W5" s="885"/>
-      <c r="X5" s="885"/>
+      <c r="W5" s="883"/>
+      <c r="X5" s="883"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31617,7 +31644,7 @@
       <c r="S19" s="147"/>
       <c r="U19" s="34"/>
       <c r="V19" s="128"/>
-      <c r="W19" s="886"/>
+      <c r="W19" s="884"/>
       <c r="X19" s="541"/>
       <c r="Y19" s="233"/>
     </row>
@@ -31671,7 +31698,7 @@
       <c r="S20" s="147"/>
       <c r="U20" s="34"/>
       <c r="V20" s="128"/>
-      <c r="W20" s="886"/>
+      <c r="W20" s="884"/>
       <c r="X20" s="34"/>
       <c r="Y20" s="233"/>
     </row>
@@ -31726,8 +31753,8 @@
       <c r="S21" s="147"/>
       <c r="U21" s="34"/>
       <c r="V21" s="128"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -31838,8 +31865,8 @@
       <c r="S23" s="147"/>
       <c r="U23" s="34"/>
       <c r="V23" s="128"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -31900,8 +31927,8 @@
       <c r="S24" s="147"/>
       <c r="U24" s="34"/>
       <c r="V24" s="128"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -31954,8 +31981,8 @@
       </c>
       <c r="U25" s="34"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -32010,8 +32037,8 @@
       <c r="T26" s="128"/>
       <c r="U26" s="34"/>
       <c r="V26" s="128"/>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -32066,9 +32093,9 @@
       <c r="T27" s="128"/>
       <c r="U27" s="34"/>
       <c r="V27" s="128"/>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32122,9 +32149,9 @@
       <c r="T28" s="128"/>
       <c r="U28" s="34"/>
       <c r="V28" s="128"/>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32708,11 +32735,11 @@
       <c r="J41" s="56"/>
       <c r="K41" s="38"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="806">
+      <c r="M41" s="795">
         <f>SUM(M5:M40)</f>
         <v>1509924.1</v>
       </c>
-      <c r="N41" s="806">
+      <c r="N41" s="795">
         <f>SUM(N5:N40)</f>
         <v>1012291</v>
       </c>
@@ -32744,8 +32771,8 @@
       <c r="L42" s="637">
         <v>3095.88</v>
       </c>
-      <c r="M42" s="807"/>
-      <c r="N42" s="807"/>
+      <c r="M42" s="796"/>
+      <c r="N42" s="796"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="861"/>
     </row>
@@ -33236,26 +33263,26 @@
       <c r="A63" s="98"/>
       <c r="B63" s="99"/>
       <c r="C63" s="1"/>
-      <c r="H63" s="761" t="s">
+      <c r="H63" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="762"/>
+      <c r="I63" s="773"/>
       <c r="J63" s="559"/>
-      <c r="K63" s="882">
+      <c r="K63" s="889">
         <f>I61+L61</f>
         <v>340912.75</v>
       </c>
-      <c r="L63" s="883"/>
+      <c r="L63" s="890"/>
       <c r="M63" s="272"/>
       <c r="N63" s="272"/>
       <c r="P63" s="34"/>
       <c r="Q63" s="13"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D64" s="767" t="s">
+      <c r="D64" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="767"/>
+      <c r="E64" s="778"/>
       <c r="F64" s="312">
         <f>F61-K63-C61</f>
         <v>1458827.53</v>
@@ -33264,22 +33291,22 @@
       <c r="J64" s="560"/>
     </row>
     <row r="65" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D65" s="797" t="s">
+      <c r="D65" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E65" s="797"/>
+      <c r="E65" s="802"/>
       <c r="F65" s="111">
         <v>-1572197.3</v>
       </c>
-      <c r="I65" s="768" t="s">
+      <c r="I65" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J65" s="769"/>
-      <c r="K65" s="770">
+      <c r="J65" s="780"/>
+      <c r="K65" s="781">
         <f>F67+F68+F69</f>
         <v>2392765.5300000003</v>
       </c>
-      <c r="L65" s="770"/>
+      <c r="L65" s="781"/>
       <c r="M65" s="404"/>
       <c r="N65" s="404"/>
       <c r="O65" s="579"/>
@@ -33320,11 +33347,11 @@
         <v>15</v>
       </c>
       <c r="J67" s="109"/>
-      <c r="K67" s="884">
+      <c r="K67" s="885">
         <f>-C4</f>
         <v>-2112071.92</v>
       </c>
-      <c r="L67" s="770"/>
+      <c r="L67" s="781"/>
     </row>
     <row r="68" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="110" t="s">
@@ -33341,22 +33368,22 @@
       <c r="C69" s="112">
         <v>44710</v>
       </c>
-      <c r="D69" s="750" t="s">
+      <c r="D69" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="751"/>
+      <c r="E69" s="762"/>
       <c r="F69" s="113">
         <v>2546982.16</v>
       </c>
-      <c r="I69" s="879" t="s">
+      <c r="I69" s="886" t="s">
         <v>198</v>
       </c>
-      <c r="J69" s="880"/>
-      <c r="K69" s="881">
+      <c r="J69" s="887"/>
+      <c r="K69" s="888">
         <f>K65+K67</f>
         <v>280693.61000000034</v>
       </c>
-      <c r="L69" s="881"/>
+      <c r="L69" s="888"/>
     </row>
     <row r="70" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C70" s="114"/>
@@ -33503,6 +33530,21 @@
     <sortCondition ref="J42:J56"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -33518,21 +33560,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K65:L65"/>
   </mergeCells>
   <pageMargins left="0.28000000000000003" right="0.19" top="0.33" bottom="0.33" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -35874,11 +35901,11 @@
       <c r="N88"/>
     </row>
     <row r="89" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="889" t="s">
+      <c r="A89" s="893" t="s">
         <v>804</v>
       </c>
-      <c r="B89" s="890"/>
-      <c r="C89" s="890"/>
+      <c r="B89" s="894"/>
+      <c r="C89" s="894"/>
       <c r="E89"/>
       <c r="F89" s="111"/>
       <c r="I89"/>
@@ -35888,10 +35915,10 @@
     </row>
     <row r="90" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="454"/>
-      <c r="B90" s="891" t="s">
+      <c r="B90" s="895" t="s">
         <v>805</v>
       </c>
-      <c r="C90" s="892"/>
+      <c r="C90" s="896"/>
       <c r="E90"/>
       <c r="F90" s="111"/>
       <c r="I90"/>
@@ -35992,7 +36019,7 @@
     <row r="97" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="658"/>
-      <c r="C97" s="887">
+      <c r="C97" s="891">
         <f>SUM(C91:C96)</f>
         <v>625124.87</v>
       </c>
@@ -36006,7 +36033,7 @@
       <c r="B98" s="659" t="s">
         <v>881</v>
       </c>
-      <c r="C98" s="888"/>
+      <c r="C98" s="892"/>
       <c r="E98"/>
       <c r="F98" s="127">
         <v>0</v>
@@ -36107,7 +36134,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>882</v>
       </c>
@@ -36123,7 +36150,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -36133,21 +36160,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -36165,14 +36192,14 @@
       <c r="D4" s="18">
         <v>44710</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -36182,7 +36209,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -37954,11 +37981,11 @@
       <c r="L41" s="39">
         <v>18992.37</v>
       </c>
-      <c r="M41" s="806">
+      <c r="M41" s="795">
         <f>SUM(M5:M40)</f>
         <v>1737024</v>
       </c>
-      <c r="N41" s="806">
+      <c r="N41" s="795">
         <f>SUM(N5:N40)</f>
         <v>1314313</v>
       </c>
@@ -37996,8 +38023,8 @@
       <c r="L42" s="52">
         <v>17035.3</v>
       </c>
-      <c r="M42" s="807"/>
-      <c r="N42" s="807"/>
+      <c r="M42" s="796"/>
+      <c r="N42" s="796"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="861"/>
     </row>
@@ -38676,26 +38703,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="761" t="s">
+      <c r="H69" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="762"/>
+      <c r="I69" s="773"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="882">
+      <c r="K69" s="889">
         <f>I67+L67</f>
         <v>534683.29</v>
       </c>
-      <c r="L69" s="883"/>
+      <c r="L69" s="890"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="767" t="s">
+      <c r="D70" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="767"/>
+      <c r="E70" s="778"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1883028.8699999999</v>
@@ -38704,22 +38731,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="797" t="s">
+      <c r="D71" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="797"/>
+      <c r="E71" s="802"/>
       <c r="F71" s="111">
         <v>-2122394.9</v>
       </c>
-      <c r="I71" s="768" t="s">
+      <c r="I71" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="769"/>
-      <c r="K71" s="770">
+      <c r="J71" s="780"/>
+      <c r="K71" s="781">
         <f>F73+F74+F75</f>
         <v>2367293.46</v>
       </c>
-      <c r="L71" s="770"/>
+      <c r="L71" s="781"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -38760,11 +38787,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="884">
+      <c r="K73" s="885">
         <f>-C4</f>
         <v>-2546982.16</v>
       </c>
-      <c r="L73" s="770"/>
+      <c r="L73" s="781"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -38781,22 +38808,22 @@
       <c r="C75" s="112">
         <v>44745</v>
       </c>
-      <c r="D75" s="750" t="s">
+      <c r="D75" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="751"/>
+      <c r="E75" s="762"/>
       <c r="F75" s="113">
         <v>2355426.54</v>
       </c>
-      <c r="I75" s="752" t="s">
+      <c r="I75" s="763" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="753"/>
-      <c r="K75" s="754">
+      <c r="J75" s="764"/>
+      <c r="K75" s="765">
         <f>K71+K73</f>
         <v>-179688.70000000019</v>
       </c>
-      <c r="L75" s="754"/>
+      <c r="L75" s="765"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -38943,17 +38970,6 @@
     <sortCondition ref="B42:B51"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="Q41:Q42"/>
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="I75:J75"/>
@@ -38965,6 +38981,17 @@
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="K71:L71"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="Q41:Q42"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44611,7 +44638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>1025</v>
       </c>
@@ -44627,7 +44654,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -44637,21 +44664,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -44669,14 +44696,14 @@
       <c r="D4" s="18">
         <v>44745</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -44686,7 +44713,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -46424,11 +46451,11 @@
       <c r="L41" s="39">
         <v>3442.5</v>
       </c>
-      <c r="M41" s="806">
+      <c r="M41" s="795">
         <f>SUM(M5:M40)</f>
         <v>2180659.5</v>
       </c>
-      <c r="N41" s="806">
+      <c r="N41" s="795">
         <f>SUM(N5:N40)</f>
         <v>1072718</v>
       </c>
@@ -46466,8 +46493,8 @@
       <c r="L42" s="702">
         <v>28000</v>
       </c>
-      <c r="M42" s="807"/>
-      <c r="N42" s="807"/>
+      <c r="M42" s="796"/>
+      <c r="N42" s="796"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="861"/>
     </row>
@@ -47071,26 +47098,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="761" t="s">
+      <c r="H69" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="762"/>
+      <c r="I69" s="773"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="882">
+      <c r="K69" s="889">
         <f>I67+L67</f>
         <v>515778.65000000026</v>
       </c>
-      <c r="L69" s="883"/>
+      <c r="L69" s="890"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="767" t="s">
+      <c r="D70" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="767"/>
+      <c r="E70" s="778"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1573910.5599999998</v>
@@ -47099,22 +47126,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="797" t="s">
+      <c r="D71" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="797"/>
+      <c r="E71" s="802"/>
       <c r="F71" s="111">
         <v>-1727771.26</v>
       </c>
-      <c r="I71" s="768" t="s">
+      <c r="I71" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="769"/>
-      <c r="K71" s="770">
+      <c r="J71" s="780"/>
+      <c r="K71" s="781">
         <f>F73+F74+F75</f>
         <v>2141254.8899999997</v>
       </c>
-      <c r="L71" s="770"/>
+      <c r="L71" s="781"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -47155,11 +47182,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="884">
+      <c r="K73" s="885">
         <f>-C4</f>
         <v>-2355426.54</v>
       </c>
-      <c r="L73" s="770"/>
+      <c r="L73" s="781"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -47176,22 +47203,22 @@
       <c r="C75" s="112">
         <v>44773</v>
       </c>
-      <c r="D75" s="750" t="s">
+      <c r="D75" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="751"/>
+      <c r="E75" s="762"/>
       <c r="F75" s="113">
         <v>2274653.09</v>
       </c>
-      <c r="I75" s="879" t="s">
+      <c r="I75" s="886" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="880"/>
-      <c r="K75" s="881">
+      <c r="J75" s="887"/>
+      <c r="K75" s="888">
         <f>K71+K73</f>
         <v>-214171.65000000037</v>
       </c>
-      <c r="L75" s="881"/>
+      <c r="L75" s="888"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -47338,6 +47365,12 @@
     <sortCondition ref="B35:B44"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -47354,12 +47387,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -49948,7 +49975,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>1142</v>
       </c>
@@ -49964,7 +49991,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -49974,21 +50001,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="553"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -50006,14 +50033,14 @@
       <c r="D4" s="18">
         <v>44773</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="556"/>
       <c r="K4" s="562"/>
       <c r="L4" s="563"/>
@@ -50023,7 +50050,7 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
@@ -51746,11 +51773,11 @@
       <c r="L41" s="39">
         <v>10440</v>
       </c>
-      <c r="M41" s="806">
+      <c r="M41" s="795">
         <f>SUM(M5:M40)</f>
         <v>1553743.1800000002</v>
       </c>
-      <c r="N41" s="806">
+      <c r="N41" s="795">
         <f>SUM(N5:N40)</f>
         <v>1198132</v>
       </c>
@@ -51786,8 +51813,8 @@
       <c r="L42" s="702">
         <v>1856</v>
       </c>
-      <c r="M42" s="807"/>
-      <c r="N42" s="807"/>
+      <c r="M42" s="796"/>
+      <c r="N42" s="796"/>
       <c r="P42" s="34"/>
       <c r="Q42" s="861"/>
       <c r="R42" s="227">
@@ -52359,26 +52386,26 @@
       <c r="A69" s="98"/>
       <c r="B69" s="99"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="761" t="s">
+      <c r="H69" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="762"/>
+      <c r="I69" s="773"/>
       <c r="J69" s="559"/>
-      <c r="K69" s="882">
+      <c r="K69" s="889">
         <f>I67+L67</f>
         <v>573073.52</v>
       </c>
-      <c r="L69" s="883"/>
+      <c r="L69" s="890"/>
       <c r="M69" s="272"/>
       <c r="N69" s="272"/>
       <c r="P69" s="34"/>
       <c r="Q69" s="13"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="767" t="s">
+      <c r="D70" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="767"/>
+      <c r="E70" s="778"/>
       <c r="F70" s="312">
         <f>F67-K69-C67</f>
         <v>1262114.75</v>
@@ -52387,22 +52414,22 @@
       <c r="J70" s="560"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="797" t="s">
+      <c r="D71" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="797"/>
+      <c r="E71" s="802"/>
       <c r="F71" s="111">
         <v>-1715125.23</v>
       </c>
-      <c r="I71" s="768" t="s">
+      <c r="I71" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J71" s="769"/>
-      <c r="K71" s="770">
+      <c r="J71" s="780"/>
+      <c r="K71" s="781">
         <f>F73+F74+F75</f>
         <v>2249865.5500000003</v>
       </c>
-      <c r="L71" s="770"/>
+      <c r="L71" s="781"/>
       <c r="M71" s="404"/>
       <c r="N71" s="404"/>
       <c r="O71" s="654"/>
@@ -52443,11 +52470,11 @@
         <v>15</v>
       </c>
       <c r="J73" s="109"/>
-      <c r="K73" s="884">
+      <c r="K73" s="885">
         <f>-C4</f>
         <v>-2274653.09</v>
       </c>
-      <c r="L73" s="770"/>
+      <c r="L73" s="781"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="110" t="s">
@@ -52464,22 +52491,22 @@
       <c r="C75" s="112">
         <v>44801</v>
       </c>
-      <c r="D75" s="750" t="s">
+      <c r="D75" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="751"/>
+      <c r="E75" s="762"/>
       <c r="F75" s="113">
         <v>2672555.9900000002</v>
       </c>
-      <c r="I75" s="752" t="s">
+      <c r="I75" s="763" t="s">
         <v>97</v>
       </c>
-      <c r="J75" s="753"/>
-      <c r="K75" s="754">
+      <c r="J75" s="764"/>
+      <c r="K75" s="765">
         <f>K71+K73</f>
         <v>-24787.539999999572</v>
       </c>
-      <c r="L75" s="754"/>
+      <c r="L75" s="765"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="114"/>
@@ -52623,6 +52650,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -52639,12 +52672,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -55074,23 +55101,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
-      <c r="C1" s="776" t="s">
+      <c r="B1" s="750"/>
+      <c r="C1" s="752" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="777"/>
-      <c r="E1" s="777"/>
-      <c r="F1" s="777"/>
-      <c r="G1" s="777"/>
-      <c r="H1" s="777"/>
-      <c r="I1" s="777"/>
-      <c r="J1" s="777"/>
-      <c r="K1" s="777"/>
-      <c r="L1" s="777"/>
-      <c r="M1" s="777"/>
+      <c r="D1" s="753"/>
+      <c r="E1" s="753"/>
+      <c r="F1" s="753"/>
+      <c r="G1" s="753"/>
+      <c r="H1" s="753"/>
+      <c r="I1" s="753"/>
+      <c r="J1" s="753"/>
+      <c r="K1" s="753"/>
+      <c r="L1" s="753"/>
+      <c r="M1" s="753"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -55100,21 +55127,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
     </row>
@@ -55129,14 +55156,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -55146,14 +55173,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -55204,8 +55231,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -55976,7 +56003,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -56028,7 +56055,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -56077,8 +56104,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -56179,8 +56206,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -56234,8 +56261,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -56281,8 +56308,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -56333,8 +56360,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -56382,9 +56409,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -56434,9 +56461,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -56771,11 +56798,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="806">
+      <c r="M36" s="795">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="808">
+      <c r="N36" s="797">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -56783,7 +56810,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="810">
+      <c r="Q36" s="799">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -56818,13 +56845,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="807"/>
-      <c r="N37" s="809"/>
+      <c r="M37" s="796"/>
+      <c r="N37" s="798"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="811"/>
+      <c r="Q37" s="800"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -57114,26 +57141,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="761" t="s">
+      <c r="H52" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="762"/>
+      <c r="I52" s="773"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="763">
+      <c r="K52" s="774">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="796"/>
+      <c r="L52" s="801"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="767" t="s">
+      <c r="D53" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="767"/>
+      <c r="E53" s="778"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -57142,29 +57169,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="797" t="s">
+      <c r="D54" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="797"/>
+      <c r="E54" s="802"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="768" t="s">
+      <c r="I54" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="769"/>
-      <c r="K54" s="770">
+      <c r="J54" s="780"/>
+      <c r="K54" s="781">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="770"/>
-      <c r="M54" s="798" t="s">
+      <c r="L54" s="781"/>
+      <c r="M54" s="787" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="799"/>
-      <c r="O54" s="799"/>
-      <c r="P54" s="799"/>
-      <c r="Q54" s="800"/>
+      <c r="N54" s="788"/>
+      <c r="O54" s="788"/>
+      <c r="P54" s="788"/>
+      <c r="Q54" s="789"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -57178,11 +57205,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="801"/>
-      <c r="N55" s="802"/>
-      <c r="O55" s="802"/>
-      <c r="P55" s="802"/>
-      <c r="Q55" s="803"/>
+      <c r="M55" s="790"/>
+      <c r="N55" s="791"/>
+      <c r="O55" s="791"/>
+      <c r="P55" s="791"/>
+      <c r="Q55" s="792"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -57200,11 +57227,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="772">
+      <c r="K56" s="783">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="773"/>
+      <c r="L56" s="784"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -57221,22 +57248,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="750" t="s">
+      <c r="D58" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="751"/>
+      <c r="E58" s="762"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="752" t="s">
+      <c r="I58" s="763" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="753"/>
-      <c r="K58" s="754">
+      <c r="J58" s="764"/>
+      <c r="K58" s="765">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="754"/>
+      <c r="L58" s="765"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -57380,17 +57407,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -57401,14 +57425,17 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -60151,23 +60178,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
-      <c r="C1" s="776" t="s">
+      <c r="B1" s="750"/>
+      <c r="C1" s="752" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="777"/>
-      <c r="E1" s="777"/>
-      <c r="F1" s="777"/>
-      <c r="G1" s="777"/>
-      <c r="H1" s="777"/>
-      <c r="I1" s="777"/>
-      <c r="J1" s="777"/>
-      <c r="K1" s="777"/>
-      <c r="L1" s="777"/>
-      <c r="M1" s="777"/>
+      <c r="D1" s="753"/>
+      <c r="E1" s="753"/>
+      <c r="F1" s="753"/>
+      <c r="G1" s="753"/>
+      <c r="H1" s="753"/>
+      <c r="I1" s="753"/>
+      <c r="J1" s="753"/>
+      <c r="K1" s="753"/>
+      <c r="L1" s="753"/>
+      <c r="M1" s="753"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -60177,21 +60204,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -60209,14 +60236,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -60226,15 +60253,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -60295,8 +60322,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -61053,7 +61080,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -61105,7 +61132,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -61154,8 +61181,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -61256,8 +61283,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -61308,8 +61335,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -61355,8 +61382,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -61404,8 +61431,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -61465,9 +61492,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -61521,9 +61548,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -61839,11 +61866,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="806">
+      <c r="M36" s="795">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="808">
+      <c r="N36" s="797">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -61851,7 +61878,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="810">
+      <c r="Q36" s="799">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -61870,13 +61897,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="807"/>
-      <c r="N37" s="809"/>
+      <c r="M37" s="796"/>
+      <c r="N37" s="798"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="811"/>
+      <c r="Q37" s="800"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -62150,26 +62177,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="761" t="s">
+      <c r="H52" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="762"/>
+      <c r="I52" s="773"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="763">
+      <c r="K52" s="774">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="796"/>
+      <c r="L52" s="801"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="767" t="s">
+      <c r="D53" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="767"/>
+      <c r="E53" s="778"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -62178,29 +62205,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="797" t="s">
+      <c r="D54" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="797"/>
+      <c r="E54" s="802"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="768" t="s">
+      <c r="I54" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="769"/>
-      <c r="K54" s="770">
+      <c r="J54" s="780"/>
+      <c r="K54" s="781">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="770"/>
-      <c r="M54" s="798" t="s">
+      <c r="L54" s="781"/>
+      <c r="M54" s="787" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="799"/>
-      <c r="O54" s="799"/>
-      <c r="P54" s="799"/>
-      <c r="Q54" s="800"/>
+      <c r="N54" s="788"/>
+      <c r="O54" s="788"/>
+      <c r="P54" s="788"/>
+      <c r="Q54" s="789"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -62214,11 +62241,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="801"/>
-      <c r="N55" s="802"/>
-      <c r="O55" s="802"/>
-      <c r="P55" s="802"/>
-      <c r="Q55" s="803"/>
+      <c r="M55" s="790"/>
+      <c r="N55" s="791"/>
+      <c r="O55" s="791"/>
+      <c r="P55" s="791"/>
+      <c r="Q55" s="792"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -62236,11 +62263,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="772">
+      <c r="K56" s="783">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="773"/>
+      <c r="L56" s="784"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -62257,22 +62284,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="750" t="s">
+      <c r="D58" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="751"/>
+      <c r="E58" s="762"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="752" t="s">
+      <c r="I58" s="763" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="753"/>
-      <c r="K58" s="754">
+      <c r="J58" s="764"/>
+      <c r="K58" s="765">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="754"/>
+      <c r="L58" s="765"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -62416,13 +62443,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -62432,20 +62466,13 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -65140,7 +65167,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>316</v>
       </c>
@@ -65156,7 +65183,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -65166,21 +65193,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -65198,14 +65225,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -65215,15 +65242,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -65274,8 +65301,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -66039,7 +66066,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -66092,7 +66119,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -66141,8 +66168,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -66242,8 +66269,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -66298,8 +66325,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -66344,8 +66371,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -66393,8 +66420,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -66448,9 +66475,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -66504,9 +66531,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -66817,11 +66844,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="806">
+      <c r="M36" s="795">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="808">
+      <c r="N36" s="797">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -66829,7 +66856,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="810">
+      <c r="Q36" s="799">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -66854,13 +66881,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="807"/>
-      <c r="N37" s="809"/>
+      <c r="M37" s="796"/>
+      <c r="N37" s="798"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="811"/>
+      <c r="Q37" s="800"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -67153,26 +67180,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="761" t="s">
+      <c r="H52" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="762"/>
+      <c r="I52" s="773"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="763">
+      <c r="K52" s="774">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="796"/>
+      <c r="L52" s="801"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="767" t="s">
+      <c r="D53" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="767"/>
+      <c r="E53" s="778"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -67181,22 +67208,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="797" t="s">
+      <c r="D54" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="797"/>
+      <c r="E54" s="802"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="768" t="s">
+      <c r="I54" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="769"/>
-      <c r="K54" s="770">
+      <c r="J54" s="780"/>
+      <c r="K54" s="781">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="770"/>
+      <c r="L54" s="781"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -67237,11 +67264,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="772">
+      <c r="K56" s="783">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="773"/>
+      <c r="L56" s="784"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -67258,22 +67285,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="750" t="s">
+      <c r="D58" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="751"/>
+      <c r="E58" s="762"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="752" t="s">
+      <c r="I58" s="763" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="753"/>
-      <c r="K58" s="754">
+      <c r="J58" s="764"/>
+      <c r="K58" s="765">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="754"/>
+      <c r="L58" s="765"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -67417,6 +67444,20 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="W27:X28"/>
@@ -67432,20 +67473,6 @@
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -70239,7 +70266,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="774"/>
+      <c r="B1" s="750"/>
       <c r="C1" s="816" t="s">
         <v>646</v>
       </c>
@@ -70255,7 +70282,7 @@
       <c r="M1" s="817"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="775"/>
+      <c r="B2" s="751"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -70265,21 +70292,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="778" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="779"/>
+      <c r="B3" s="754" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="755"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="780" t="s">
+      <c r="H3" s="756" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="780"/>
+      <c r="I3" s="756"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="804" t="s">
+      <c r="P3" s="793" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="814" t="s">
@@ -70297,14 +70324,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="781" t="s">
+      <c r="E4" s="757" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="782"/>
-      <c r="H4" s="783" t="s">
+      <c r="F4" s="758"/>
+      <c r="H4" s="759" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="784"/>
+      <c r="I4" s="760"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -70314,15 +70341,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="805"/>
+      <c r="P4" s="794"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="815"/>
-      <c r="W4" s="787" t="s">
+      <c r="W4" s="803" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="787"/>
+      <c r="X4" s="803"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -70373,8 +70400,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="787"/>
-      <c r="X5" s="787"/>
+      <c r="W5" s="803"/>
+      <c r="X5" s="803"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -71135,7 +71162,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="791">
+      <c r="W19" s="807">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -71187,7 +71214,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="792"/>
+      <c r="W20" s="808"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -71236,8 +71263,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="793"/>
-      <c r="X21" s="793"/>
+      <c r="W21" s="809"/>
+      <c r="X21" s="809"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -71336,8 +71363,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="794"/>
-      <c r="X23" s="794"/>
+      <c r="W23" s="810"/>
+      <c r="X23" s="810"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -71392,8 +71419,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="794"/>
-      <c r="X24" s="794"/>
+      <c r="W24" s="810"/>
+      <c r="X24" s="810"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -71441,8 +71468,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="795"/>
-      <c r="X25" s="795"/>
+      <c r="W25" s="811"/>
+      <c r="X25" s="811"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -71490,8 +71517,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="795"/>
-      <c r="X26" s="795"/>
+      <c r="W26" s="811"/>
+      <c r="X26" s="811"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -71539,9 +71566,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="788"/>
-      <c r="X27" s="789"/>
-      <c r="Y27" s="790"/>
+      <c r="W27" s="804"/>
+      <c r="X27" s="805"/>
+      <c r="Y27" s="806"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -71589,9 +71616,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="789"/>
-      <c r="X28" s="789"/>
-      <c r="Y28" s="790"/>
+      <c r="W28" s="805"/>
+      <c r="X28" s="805"/>
+      <c r="Y28" s="806"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -71932,11 +71959,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="806">
+      <c r="M36" s="795">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="808">
+      <c r="N36" s="797">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -71969,8 +71996,8 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="807"/>
-      <c r="N37" s="809"/>
+      <c r="M37" s="796"/>
+      <c r="N37" s="798"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
@@ -72277,26 +72304,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="761" t="s">
+      <c r="H52" s="772" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="762"/>
+      <c r="I52" s="773"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="763">
+      <c r="K52" s="774">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="796"/>
+      <c r="L52" s="801"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="767" t="s">
+      <c r="D53" s="778" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="767"/>
+      <c r="E53" s="778"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -72305,22 +72332,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="797" t="s">
+      <c r="D54" s="802" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="797"/>
+      <c r="E54" s="802"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="768" t="s">
+      <c r="I54" s="779" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="769"/>
-      <c r="K54" s="770">
+      <c r="J54" s="780"/>
+      <c r="K54" s="781">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="770"/>
+      <c r="L54" s="781"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -72361,11 +72388,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="772">
+      <c r="K56" s="783">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="773"/>
+      <c r="L56" s="784"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -72382,22 +72409,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="750" t="s">
+      <c r="D58" s="761" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="751"/>
+      <c r="E58" s="762"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="752" t="s">
+      <c r="I58" s="763" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="753"/>
-      <c r="K58" s="754">
+      <c r="J58" s="764"/>
+      <c r="K58" s="765">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="754"/>
+      <c r="L58" s="765"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -72541,20 +72568,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -72571,6 +72584,20 @@
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="M39:N39"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
   </mergeCells>
   <pageMargins left="0.23" right="0.23" top="0.4" bottom="0.28000000000000003" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>